<commit_message>
EcoTrack-FrontEnd V0.2 intergrate components into info page BackEnd add db config route and models
</commit_message>
<xml_diff>
--- a/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
+++ b/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marsh\Documents\Calculator\InfosysEcoTrack\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rick/Git/EcoTrackFront-End/ecotrack-backend/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0EA96AC-1A72-4FD0-B632-70618F02777F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2318F48B-CC7F-574D-B86A-BDE8EAB5D292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity" sheetId="1" r:id="rId1"/>
@@ -848,15 +848,9 @@
     <t>South Australia</t>
   </si>
   <si>
-    <t>Western Australia -</t>
-  </si>
-  <si>
     <t>Tasmania</t>
   </si>
   <si>
-    <t>Northern territory -</t>
-  </si>
-  <si>
     <t>National</t>
   </si>
   <si>
@@ -867,6 +861,12 @@
   </si>
   <si>
     <t>South West Interconnected System (SWIS)</t>
+  </si>
+  <si>
+    <t>Western Australia</t>
+  </si>
+  <si>
+    <t>Northern territory</t>
   </si>
 </sst>
 </file>
@@ -1513,6 +1513,18 @@
     <xf numFmtId="3" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1524,18 +1536,6 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1893,33 +1893,33 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="48" t="s">
+      <c r="C1" s="53"/>
+      <c r="D1" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="49"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
+      <c r="E1" s="53"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="51"/>
       <c r="B2" s="41" t="s">
         <v>108</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>110</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>111</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>112</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>113</v>
       </c>
@@ -2001,35 +2001,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="46">
+        <v>0.51</v>
+      </c>
+      <c r="C7" s="48">
+        <v>164</v>
+      </c>
+      <c r="D7" s="46">
+        <v>0.04</v>
+      </c>
+      <c r="E7" s="48">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B8" s="47"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="49"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="B7" s="50">
-        <v>0.51</v>
-      </c>
-      <c r="C7" s="52">
-        <v>164</v>
-      </c>
-      <c r="D7" s="50">
-        <v>0.04</v>
-      </c>
-      <c r="E7" s="52">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="53"/>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="B9" s="5">
         <v>0.17</v>
@@ -2044,35 +2044,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="46">
+        <v>0.54</v>
+      </c>
+      <c r="C10" s="48">
+        <v>152</v>
+      </c>
+      <c r="D10" s="46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E10" s="48">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="49"/>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B10" s="50">
-        <v>0.54</v>
-      </c>
-      <c r="C10" s="52">
-        <v>152</v>
-      </c>
-      <c r="D10" s="50">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E10" s="52">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="53"/>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="B12" s="5">
         <v>0.57999999999999996</v>
@@ -2087,9 +2087,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="44" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B13" s="27">
         <v>0.68</v>
@@ -2131,15 +2131,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="39" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5" style="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="54" t="s">
         <v>34</v>
       </c>
@@ -2153,7 +2153,7 @@
       <c r="E1" s="57"/>
       <c r="F1" s="58"/>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="55"/>
       <c r="B2" s="32" t="s">
         <v>88</v>
@@ -2171,7 +2171,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>89</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>90</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>51.63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>91</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>92</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>93</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>94</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>56.56</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>95</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>37.08</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>96</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>234.05</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>97</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>60.27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>98</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>100</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>101</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>102</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>103</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>104</v>
       </c>
@@ -2489,19 +2489,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" style="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="50" t="s">
         <v>35</v>
       </c>
       <c r="C1" s="61" t="s">
@@ -2514,7 +2514,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="59"/>
       <c r="B2" s="59"/>
       <c r="C2" s="64" t="s">
@@ -2527,7 +2527,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="60"/>
       <c r="B3" s="60"/>
       <c r="C3" s="67"/>
@@ -2536,7 +2536,7 @@
       <c r="F3" s="69"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
         <v>40</v>
@@ -2557,7 +2557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>46</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>48</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>49</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
         <v>52</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>54</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>56</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>58</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>60</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>62</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>64</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>66</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>68</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>70</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
         <v>71</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
         <v>73</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
         <v>75</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>77</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
         <v>79</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
         <v>80</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>81</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
         <v>83</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="24" t="s">
         <v>85</v>
       </c>
@@ -3084,14 +3084,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>19</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -3113,7 +3113,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
@@ -3124,7 +3124,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>29</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
         <v>31</v>
       </c>
@@ -3212,7 +3212,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>33</v>
       </c>
@@ -3248,13 +3248,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>0.1229</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>0.3276</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>8.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -3316,13 +3316,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -3338,7 +3338,7 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>2.931</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>1.649</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -3384,13 +3384,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
EcoTrack V0.2 finished the elec prototype
</commit_message>
<xml_diff>
--- a/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
+++ b/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rick/Git/EcoTrackFront-End/ecotrack-backend/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2318F48B-CC7F-574D-B86A-BDE8EAB5D292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{807B49EC-B39E-7A4E-BD76-55125050B66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -866,7 +866,7 @@
     <t>Western Australia</t>
   </si>
   <si>
-    <t>Northern territory</t>
+    <t>Northern Territory</t>
   </si>
 </sst>
 </file>
@@ -1893,7 +1893,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
solid fuels commit 2nd
</commit_message>
<xml_diff>
--- a/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
+++ b/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
@@ -1,34 +1,76 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marsh\Documents\Calculator\EcoTrackFront-End\ecotrack-backend\Documentation\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A517E1B9-09A5-4A3F-8289-63F55C3F9630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Electricity" sheetId="1" r:id="rId1"/>
-    <sheet name="Solid Fuel" sheetId="9" r:id="rId2"/>
-    <sheet name="Gaseous Fuel" sheetId="2" r:id="rId3"/>
-    <sheet name="Liquid Fuel" sheetId="3" r:id="rId4"/>
-    <sheet name="Solid Waste" sheetId="4" r:id="rId5"/>
-    <sheet name="Wastewater Treatment" sheetId="5" r:id="rId6"/>
-    <sheet name="Biological Treatment" sheetId="7" r:id="rId7"/>
-    <sheet name="Waste Incineration" sheetId="6" r:id="rId8"/>
+    <sheet r:id="rId1" sheetId="1" name="Electricity"/>
+    <sheet r:id="rId2" sheetId="2" name="Solid Fuel"/>
+    <sheet r:id="rId3" sheetId="3" name="Gaseous Fuel"/>
+    <sheet r:id="rId4" sheetId="4" name="Liquid Fuel"/>
+    <sheet r:id="rId5" sheetId="5" name="Solid Waste"/>
+    <sheet r:id="rId6" sheetId="6" name="Wastewater Treatment"/>
+    <sheet r:id="rId7" sheetId="7" name="Biological Treatment"/>
+    <sheet r:id="rId8" sheetId="8" name="Waste Incineration"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="151">
   <si>
+    <t xml:space="preserve">Waste type </t>
+  </si>
+  <si>
+    <r>
+      <t>Emission factors (t CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-e/t)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinical Waste </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sewage Sludge </t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fossil Liquid </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industrial Waste </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Municipal Solid Waste </t>
+  </si>
+  <si>
     <t xml:space="preserve">Waste treatment type  </t>
   </si>
   <si>
@@ -39,7 +81,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -50,7 +92,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -65,7 +107,7 @@
     <t>Anaerobic digestion</t>
   </si>
   <si>
-    <t xml:space="preserve">Waste type </t>
+    <t>Wastewater Treatment Method</t>
   </si>
   <si>
     <r>
@@ -75,7 +117,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -86,7 +128,52 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-e per person)</t>
+    </r>
+  </si>
+  <si>
+    <t>Managed aerobic treatment</t>
+  </si>
+  <si>
+    <t>Unmanaged aerobic treatment</t>
+  </si>
+  <si>
+    <t>Anaerobic digester/reactor</t>
+  </si>
+  <si>
+    <t>Anaerobic lagoon shallow (&lt;2 metres)</t>
+  </si>
+  <si>
+    <t>Anaerobic lagoon deep (&gt;2 metres)</t>
+  </si>
+  <si>
+    <t>Waste types</t>
+  </si>
+  <si>
+    <r>
+      <t>Scope 3 emission factor (t CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -95,35 +182,87 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Clinical Waste </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sewage Sludge </t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fossil Liquid </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Industrial Waste </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Municipal Solid Waste </t>
-  </si>
-  <si>
-    <t>Wastewater Treatment Method</t>
-  </si>
-  <si>
-    <r>
-      <t>Emission factors (t CO</t>
+    <r>
+      <t>Volume to mass conversion factor (t/m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Paper and cardboard</t>
+  </si>
+  <si>
+    <t>Garden and green</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Textiles</t>
+  </si>
+  <si>
+    <t>Sludge</t>
+  </si>
+  <si>
+    <t>Nappies</t>
+  </si>
+  <si>
+    <t>Rubber and leather</t>
+  </si>
+  <si>
+    <t>Inert waste (including concrete/metal/plastics/glass)</t>
+  </si>
+  <si>
+    <t>Municipal solid waste</t>
+  </si>
+  <si>
+    <t>Commercial and industrial waste</t>
+  </si>
+  <si>
+    <t>Construction and demolition waste</t>
+  </si>
+  <si>
+    <t>Fuel combusted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy content factor </t>
+  </si>
+  <si>
+    <t>Scope 1 Emission factor</t>
+  </si>
+  <si>
+    <t>Scope 3</t>
+  </si>
+  <si>
+    <r>
+      <t>(kg CO</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -134,141 +273,61 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-e per person)</t>
-    </r>
-  </si>
-  <si>
-    <t>Managed aerobic treatment</t>
-  </si>
-  <si>
-    <t>Unmanaged aerobic treatment</t>
-  </si>
-  <si>
-    <t>Anaerobic digester/reactor</t>
-  </si>
-  <si>
-    <t>Anaerobic lagoon shallow (&lt;2 metres)</t>
-  </si>
-  <si>
-    <t>Anaerobic lagoon deep (&gt;2 metres)</t>
-  </si>
-  <si>
-    <t>Waste types</t>
-  </si>
-  <si>
-    <r>
-      <t>Scope 3 emission factor (t CO</t>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>‑e/GJ)</t>
+    </r>
+  </si>
+  <si>
+    <t>Emission factor</t>
+  </si>
+  <si>
+    <t>(GJ per unit of fuel)</t>
+  </si>
+  <si>
+    <r>
+      <t>CO</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>2</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>CH</t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>-e/t)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Volume to mass conversion factor (t/m</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>Paper and cardboard</t>
-  </si>
-  <si>
-    <t>Garden and green</t>
-  </si>
-  <si>
-    <t>Wood</t>
-  </si>
-  <si>
-    <t>Textiles</t>
-  </si>
-  <si>
-    <t>Sludge</t>
-  </si>
-  <si>
-    <t>Nappies</t>
-  </si>
-  <si>
-    <t>Rubber and leather</t>
-  </si>
-  <si>
-    <t>Inert waste (including concrete/metal/plastics/glass)</t>
-  </si>
-  <si>
-    <t>Municipal solid waste</t>
-  </si>
-  <si>
-    <t>Commercial and industrial waste</t>
-  </si>
-  <si>
-    <t>Construction and demolition waste</t>
-  </si>
-  <si>
-    <t>Fuel combusted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy content factor </t>
-  </si>
-  <si>
-    <t>Scope 1 Emission factor</t>
-  </si>
-  <si>
-    <t>Scope 3</t>
-  </si>
-  <si>
-    <r>
-      <t>(kg CO</t>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -279,102 +338,37 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>‑e/GJ)</t>
-    </r>
-  </si>
-  <si>
-    <t>Emission factor</t>
-  </si>
-  <si>
-    <t>(GJ per unit of fuel)</t>
-  </si>
-  <si>
-    <r>
-      <t>CO</t>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>O</t>
+    </r>
+  </si>
+  <si>
+    <t>Combined gases</t>
+  </si>
+  <si>
+    <r>
+      <t>kg CO</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>2</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>CH</t>
-    </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>O</t>
-    </r>
-  </si>
-  <si>
-    <t>Combined gases</t>
-  </si>
-  <si>
-    <r>
-      <t>kg CO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -682,7 +676,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -693,7 +687,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -708,7 +702,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -719,7 +713,7 @@
       <rPr>
         <b/>
         <sz val="8"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -776,6 +770,205 @@
     <t>Biomethane</t>
   </si>
   <si>
+    <t>Solid Fuels combusted</t>
+  </si>
+  <si>
+    <t>Energy Content factor</t>
+  </si>
+  <si>
+    <r>
+      <t>Scope 1 Emission Factor  (kg CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>‑e/GJ)</t>
+    </r>
+  </si>
+  <si>
+    <t>Scope 3 Emission Factor</t>
+  </si>
+  <si>
+    <t>GJ/t</t>
+  </si>
+  <si>
+    <r>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CH</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">O </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Combined gases </t>
+  </si>
+  <si>
+    <r>
+      <t>kg CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFffffff"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">‑e /GJ </t>
+    </r>
+  </si>
+  <si>
+    <t>Bituminous coal</t>
+  </si>
+  <si>
+    <t>Sub-bituminous coal</t>
+  </si>
+  <si>
+    <t>Anthracite</t>
+  </si>
+  <si>
+    <t>Brown coal (lignite)</t>
+  </si>
+  <si>
+    <t>Coking coal</t>
+  </si>
+  <si>
+    <t>Coal briquettes</t>
+  </si>
+  <si>
+    <t>Coal coke</t>
+  </si>
+  <si>
+    <t>Coal tar</t>
+  </si>
+  <si>
+    <t>Solid fossil fuels other than those mentioned in the items above</t>
+  </si>
+  <si>
+    <t>Industrial materials that are derived from fossil fuels, if recycled and combusted to produce heat or electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Passenger car tyres, if recycled and combusted to produce heat or electricity  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Truck and off-road tyres, if recycled and combusted to produce heat or electricity </t>
+  </si>
+  <si>
+    <t>Non‑biomass municipal materials, if combusted to produce heat or electricity</t>
+  </si>
+  <si>
+    <t>Dry wood</t>
+  </si>
+  <si>
+    <t>Green and air dried wood</t>
+  </si>
+  <si>
+    <t>Sulphite lyes</t>
+  </si>
+  <si>
+    <t>Bagasse</t>
+  </si>
+  <si>
+    <t>Biomass, municipal and industrial materials, if combusted to produce heat or electricity</t>
+  </si>
+  <si>
+    <t>Charcoal</t>
+  </si>
+  <si>
+    <t>Primary solid biomass fuels other than those mentioned in the items above</t>
+  </si>
+  <si>
     <t>State, Territory or grid description</t>
   </si>
   <si>
@@ -792,7 +985,7 @@
       <rPr>
         <b/>
         <sz val="9"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Times New Roman"/>
         <family val="2"/>
       </rPr>
@@ -802,7 +995,7 @@
       <rPr>
         <b/>
         <sz val="9"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -818,7 +1011,7 @@
       <rPr>
         <b/>
         <sz val="9"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Times New Roman"/>
         <family val="2"/>
       </rPr>
@@ -828,7 +1021,7 @@
       <rPr>
         <b/>
         <sz val="9"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -868,217 +1061,14 @@
   </si>
   <si>
     <t>National</t>
-  </si>
-  <si>
-    <t>Solid fossil fuels other than those mentioned in the items above</t>
-  </si>
-  <si>
-    <t>Industrial materials that are derived from fossil fuels, if recycled and combusted to produce heat or electricity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Passenger car tyres, if recycled and combusted to produce heat or electricity  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Truck and off-road tyres, if recycled and combusted to produce heat or electricity </t>
-  </si>
-  <si>
-    <t>Non‑biomass municipal materials, if combusted to produce heat or electricity</t>
-  </si>
-  <si>
-    <t>Dry wood</t>
-  </si>
-  <si>
-    <t>Green and air dried wood</t>
-  </si>
-  <si>
-    <t>Sulphite lyes</t>
-  </si>
-  <si>
-    <t>Bagasse</t>
-  </si>
-  <si>
-    <t>Biomass, municipal and industrial materials, if combusted to produce heat or electricity</t>
-  </si>
-  <si>
-    <t>Charcoal</t>
-  </si>
-  <si>
-    <t>Primary solid biomass fuels other than those mentioned in the items above</t>
-  </si>
-  <si>
-    <t>Solid Fuels combusted</t>
-  </si>
-  <si>
-    <t>Energy Content factor</t>
-  </si>
-  <si>
-    <r>
-      <t>Scope 1 Emission Factor  (kg CO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>‑e/GJ)</t>
-    </r>
-  </si>
-  <si>
-    <t>Scope 3 Emission Factor</t>
-  </si>
-  <si>
-    <t>GJ/t</t>
-  </si>
-  <si>
-    <r>
-      <t>CO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">2 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>CH</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">O </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Combined gases </t>
-  </si>
-  <si>
-    <r>
-      <t>kg CO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">‑e /GJ </t>
-    </r>
-  </si>
-  <si>
-    <t>Bituminous coal</t>
-  </si>
-  <si>
-    <t>Sub-bituminous coal</t>
-  </si>
-  <si>
-    <t>Anthracite</t>
-  </si>
-  <si>
-    <t>Brown coal (lignite)</t>
-  </si>
-  <si>
-    <t>Coking coal</t>
-  </si>
-  <si>
-    <t>Coal briquettes</t>
-  </si>
-  <si>
-    <t>Coal coke</t>
-  </si>
-  <si>
-    <t>Coal tar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1089,7 +1079,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFffffff"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1102,7 +1092,7 @@
     <font>
       <b/>
       <sz val="9"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFffffff"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1121,81 +1111,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFffffff"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFffffff"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Times New Roman"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1204,33 +1138,21 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF083A42"/>
+        <fgColor rgb="FF083a42"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFffffff"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE2F1EE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE2F1EE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF083A42"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFe2f1ee"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1240,347 +1162,347 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="thick">
-        <color rgb="FF55AD9F"/>
+        <color rgb="FF55ad9f"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="thick">
-        <color rgb="FF55AD9F"/>
+        <color rgb="FF55ad9f"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thick">
-        <color rgb="FF55AD9F"/>
+        <color rgb="FF55ad9f"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thick">
-        <color rgb="FF55AD9F"/>
+        <color rgb="FF55ad9f"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top/>
       <bottom/>
@@ -1588,335 +1510,278 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </left>
       <right style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </right>
       <top style="medium">
-        <color rgb="FF8EC8BF"/>
+        <color rgb="FF8ec8bf"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF8EC8BF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF8EC8BF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF8EC8BF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF8EC8BF"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF8EC8BF"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF8EC8BF"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF8EC8BF"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="83">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="15" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="21" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="22" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="23" applyBorder="1" fontId="6" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="23" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="23" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="7" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="19" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="7" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="20" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="22" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="23" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="23" applyBorder="1" fontId="8" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="24" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="25" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="25" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="17" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1927,10 +1792,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1968,71 +1833,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2060,7 +1925,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -2083,11 +1948,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -2096,13 +1961,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2112,7 +1977,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -2121,7 +1986,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2130,7 +1995,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2138,10 +2003,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -2206,56 +2071,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="39" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="39" width="9.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="46"/>
-      <c r="D1" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="46"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="30.75" customFormat="1" s="1">
+      <c r="A1" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="71" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="72"/>
+      <c r="D1" s="71" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="72"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="30.75" customFormat="1" s="1">
+      <c r="A2" s="73"/>
+      <c r="B2" s="74" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="74" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="75" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="74.25" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="B3" s="5">
         <v>0.73</v>
@@ -2270,9 +2133,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A4" s="4" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="B4" s="5">
         <v>0.85</v>
@@ -2281,15 +2144,15 @@
         <v>238</v>
       </c>
       <c r="D4" s="5">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="E4" s="11">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A5" s="4" t="s">
-        <v>112</v>
+        <v>142</v>
       </c>
       <c r="B5" s="5">
         <v>0.73</v>
@@ -2304,9 +2167,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A6" s="4" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="B6" s="5">
         <v>0.25</v>
@@ -2321,35 +2184,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="47">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="33.75" customFormat="1" s="1">
+      <c r="A7" s="76" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="77">
         <v>0.51</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="78">
         <v>164</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="77">
         <v>0.04</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="78">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="60" customFormat="1" s="1">
       <c r="A8" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="50"/>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="B8" s="79"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="80"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A9" s="4" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="B9" s="5">
         <v>0.17</v>
@@ -2364,38 +2227,38 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="47">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="33.75" customFormat="1" s="1">
+      <c r="A10" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="77">
         <v>0.54</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="78">
         <v>152</v>
       </c>
-      <c r="D10" s="47">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E10" s="49">
+      <c r="D10" s="77">
+        <v>0.07</v>
+      </c>
+      <c r="E10" s="78">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="73.5" customFormat="1" s="1">
       <c r="A11" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="50"/>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="B11" s="79"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="80"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="101.25" customFormat="1" s="1">
       <c r="A12" s="4" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
       <c r="B12" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="C12" s="11">
         <v>160</v>
@@ -2407,29 +2270,25 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="26">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A13" s="81" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="38">
         <v>0.68</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="82">
         <v>189</v>
       </c>
-      <c r="D13" s="26">
+      <c r="D13" s="38">
         <v>0.09</v>
       </c>
-      <c r="E13" s="42">
+      <c r="E13" s="82">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
@@ -2437,76 +2296,90 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04BD6277-55CD-4981-91A6-80DFE3333B27}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="70" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="39" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="39" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
-        <v>133</v>
-      </c>
-      <c r="B1" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="78" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="82" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="74"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="83"/>
-    </row>
-    <row r="3" spans="1:7" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="75"/>
-      <c r="B3" s="71" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="71" t="s">
-        <v>138</v>
-      </c>
-      <c r="D3" s="71" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="F3" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="72" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="67" t="s">
-        <v>143</v>
-      </c>
-      <c r="B4" s="68">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="23.625" customFormat="1" s="1">
+      <c r="A1" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="58" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="23.625" customFormat="1" s="1">
+      <c r="A2" s="59"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="64"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33.75" customFormat="1" s="1">
+      <c r="A3" s="65"/>
+      <c r="B3" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="33" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="32.25" customFormat="1" s="1">
+      <c r="A4" s="66" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="67">
         <v>27</v>
       </c>
-      <c r="C4" s="68">
+      <c r="C4" s="67">
         <v>90</v>
       </c>
       <c r="D4" s="68">
@@ -2515,21 +2388,21 @@
       <c r="E4" s="68">
         <v>0.2</v>
       </c>
-      <c r="F4" s="70">
+      <c r="F4" s="38">
         <v>90.24</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="67">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="68">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="45" customFormat="1" s="1">
+      <c r="A5" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="67">
         <v>21</v>
       </c>
-      <c r="C5" s="68">
+      <c r="C5" s="67">
         <v>90</v>
       </c>
       <c r="D5" s="68">
@@ -2538,21 +2411,21 @@
       <c r="E5" s="68">
         <v>0.2</v>
       </c>
-      <c r="F5" s="70">
+      <c r="F5" s="38">
         <v>90.24</v>
       </c>
       <c r="G5" s="68">
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="68">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A6" s="66" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="67">
         <v>29</v>
       </c>
-      <c r="C6" s="68">
+      <c r="C6" s="67">
         <v>90</v>
       </c>
       <c r="D6" s="68">
@@ -2561,19 +2434,19 @@
       <c r="E6" s="68">
         <v>0.2</v>
       </c>
-      <c r="F6" s="70">
+      <c r="F6" s="38">
         <v>90.24</v>
       </c>
       <c r="G6" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="67" t="s">
-        <v>146</v>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="32.25" customFormat="1" s="1">
+      <c r="A7" s="66" t="s">
+        <v>118</v>
       </c>
       <c r="B7" s="68">
-        <v>10.199999999999999</v>
+        <v>10.2</v>
       </c>
       <c r="C7" s="68">
         <v>93.5</v>
@@ -2584,18 +2457,18 @@
       <c r="E7" s="68">
         <v>0.3</v>
       </c>
-      <c r="F7" s="70">
+      <c r="F7" s="38">
         <v>93.82</v>
       </c>
       <c r="G7" s="68">
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="67" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="68">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A8" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="67">
         <v>30</v>
       </c>
       <c r="C8" s="68">
@@ -2607,21 +2480,21 @@
       <c r="E8" s="68">
         <v>0.2</v>
       </c>
-      <c r="F8" s="70">
+      <c r="F8" s="38">
         <v>92.03</v>
       </c>
       <c r="G8" s="68">
         <v>6.4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="67" t="s">
-        <v>148</v>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="32.25" customFormat="1" s="1">
+      <c r="A9" s="66" t="s">
+        <v>120</v>
       </c>
       <c r="B9" s="68">
         <v>22.1</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="67">
         <v>95</v>
       </c>
       <c r="D9" s="68">
@@ -2630,21 +2503,21 @@
       <c r="E9" s="68">
         <v>0.3</v>
       </c>
-      <c r="F9" s="70">
+      <c r="F9" s="38">
         <v>95.38</v>
       </c>
       <c r="G9" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="67" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="68">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A10" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="67">
         <v>27</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="67">
         <v>107</v>
       </c>
       <c r="D10" s="68">
@@ -2653,16 +2526,16 @@
       <c r="E10" s="68">
         <v>0.2</v>
       </c>
-      <c r="F10" s="70">
+      <c r="F10" s="38">
         <v>107.23</v>
       </c>
       <c r="G10" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="67" t="s">
-        <v>150</v>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A11" s="66" t="s">
+        <v>122</v>
       </c>
       <c r="B11" s="68">
         <v>37.5</v>
@@ -2676,30 +2549,30 @@
       <c r="E11" s="68">
         <v>0.2</v>
       </c>
-      <c r="F11" s="70">
+      <c r="F11" s="38">
         <v>82.03</v>
       </c>
       <c r="G11" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A12" s="66"/>
       <c r="B12" s="68"/>
-      <c r="C12" s="68"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
+      <c r="E12" s="67"/>
       <c r="F12" s="69"/>
       <c r="G12" s="68"/>
     </row>
-    <row r="13" spans="1:7" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="67" t="s">
-        <v>121</v>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="83.25" customFormat="1" s="1">
+      <c r="A13" s="66" t="s">
+        <v>123</v>
       </c>
       <c r="B13" s="68">
         <v>22.1</v>
       </c>
-      <c r="C13" s="68">
+      <c r="C13" s="67">
         <v>95</v>
       </c>
       <c r="D13" s="68">
@@ -2708,22 +2581,22 @@
       <c r="E13" s="68">
         <v>0.2</v>
       </c>
-      <c r="F13" s="70">
+      <c r="F13" s="38">
         <v>95.28</v>
       </c>
       <c r="G13" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="240.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="67" t="s">
-        <v>122</v>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="121.5" customFormat="1" s="1">
+      <c r="A14" s="66" t="s">
+        <v>124</v>
       </c>
       <c r="B14" s="68">
         <v>26.3</v>
       </c>
       <c r="C14" s="68">
-        <v>81.599999999999994</v>
+        <v>81.6</v>
       </c>
       <c r="D14" s="68">
         <v>0.03</v>
@@ -2731,18 +2604,18 @@
       <c r="E14" s="68">
         <v>0.2</v>
       </c>
-      <c r="F14" s="70">
+      <c r="F14" s="38">
         <v>81.83</v>
       </c>
       <c r="G14" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="67" t="s">
-        <v>123</v>
-      </c>
-      <c r="B15" s="68">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="83.25" customFormat="1" s="1">
+      <c r="A15" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="67">
         <v>32</v>
       </c>
       <c r="C15" s="68">
@@ -2754,16 +2627,16 @@
       <c r="E15" s="68">
         <v>0.2</v>
       </c>
-      <c r="F15" s="70">
+      <c r="F15" s="38">
         <v>63.03</v>
       </c>
       <c r="G15" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="67" t="s">
-        <v>124</v>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="83.25" customFormat="1" s="1">
+      <c r="A16" s="66" t="s">
+        <v>126</v>
       </c>
       <c r="B16" s="68">
         <v>27.1</v>
@@ -2777,16 +2650,16 @@
       <c r="E16" s="68">
         <v>0.2</v>
       </c>
-      <c r="F16" s="70">
+      <c r="F16" s="38">
         <v>56.13</v>
       </c>
       <c r="G16" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="67" t="s">
-        <v>125</v>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="83.25" customFormat="1" s="1">
+      <c r="A17" s="66" t="s">
+        <v>127</v>
       </c>
       <c r="B17" s="68">
         <v>10.5</v>
@@ -2797,70 +2670,70 @@
       <c r="D17" s="68">
         <v>0.8</v>
       </c>
-      <c r="E17" s="68">
+      <c r="E17" s="67">
         <v>1</v>
       </c>
-      <c r="F17" s="70">
+      <c r="F17" s="38">
         <v>88.9</v>
       </c>
       <c r="G17" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="67" t="s">
-        <v>126</v>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A18" s="66" t="s">
+        <v>128</v>
       </c>
       <c r="B18" s="68">
         <v>16.2</v>
       </c>
-      <c r="C18" s="68">
+      <c r="C18" s="67">
         <v>0</v>
       </c>
       <c r="D18" s="68">
         <v>0.1</v>
       </c>
       <c r="E18" s="68">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F18" s="70">
+        <v>1.1</v>
+      </c>
+      <c r="F18" s="38">
         <v>1.2</v>
       </c>
       <c r="G18" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="67" t="s">
-        <v>127</v>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="32.25" customFormat="1" s="1">
+      <c r="A19" s="66" t="s">
+        <v>129</v>
       </c>
       <c r="B19" s="68">
         <v>10.4</v>
       </c>
-      <c r="C19" s="68">
+      <c r="C19" s="67">
         <v>0</v>
       </c>
       <c r="D19" s="68">
         <v>0.1</v>
       </c>
       <c r="E19" s="68">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F19" s="70">
+        <v>1.1</v>
+      </c>
+      <c r="F19" s="38">
         <v>1.2</v>
       </c>
       <c r="G19" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="67" t="s">
-        <v>128</v>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A20" s="66" t="s">
+        <v>130</v>
       </c>
       <c r="B20" s="68">
         <v>12.4</v>
       </c>
-      <c r="C20" s="68">
+      <c r="C20" s="67">
         <v>0</v>
       </c>
       <c r="D20" s="68">
@@ -2869,99 +2742,99 @@
       <c r="E20" s="68">
         <v>0.5</v>
       </c>
-      <c r="F20" s="70">
-        <v>0.57999999999999996</v>
+      <c r="F20" s="38">
+        <v>0.58</v>
       </c>
       <c r="G20" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="67" t="s">
-        <v>129</v>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A21" s="66" t="s">
+        <v>131</v>
       </c>
       <c r="B21" s="68">
         <v>9.6</v>
       </c>
-      <c r="C21" s="68">
+      <c r="C21" s="67">
         <v>0</v>
       </c>
       <c r="D21" s="68">
         <v>0.3</v>
       </c>
       <c r="E21" s="68">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F21" s="70">
+        <v>1.1</v>
+      </c>
+      <c r="F21" s="38">
         <v>1.4</v>
       </c>
       <c r="G21" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="195.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="67" t="s">
-        <v>130</v>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="96" customFormat="1" s="1">
+      <c r="A22" s="66" t="s">
+        <v>132</v>
       </c>
       <c r="B22" s="68">
         <v>12.2</v>
       </c>
-      <c r="C22" s="68">
+      <c r="C22" s="67">
         <v>0</v>
       </c>
       <c r="D22" s="68">
         <v>0.8</v>
       </c>
-      <c r="E22" s="68">
+      <c r="E22" s="67">
         <v>1</v>
       </c>
-      <c r="F22" s="70">
+      <c r="F22" s="38">
         <v>1.8</v>
       </c>
       <c r="G22" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="67" t="s">
-        <v>131</v>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A23" s="66" t="s">
+        <v>133</v>
       </c>
       <c r="B23" s="68">
         <v>31.1</v>
       </c>
-      <c r="C23" s="68">
+      <c r="C23" s="67">
         <v>0</v>
       </c>
       <c r="D23" s="68">
         <v>5.3</v>
       </c>
-      <c r="E23" s="68">
+      <c r="E23" s="67">
         <v>1</v>
       </c>
-      <c r="F23" s="70">
+      <c r="F23" s="38">
         <v>6.3</v>
       </c>
       <c r="G23" s="68" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="67" t="s">
-        <v>132</v>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="96" customFormat="1" s="1">
+      <c r="A24" s="66" t="s">
+        <v>134</v>
       </c>
       <c r="B24" s="68">
         <v>12.2</v>
       </c>
-      <c r="C24" s="68">
+      <c r="C24" s="67">
         <v>0</v>
       </c>
       <c r="D24" s="68">
         <v>0.8</v>
       </c>
-      <c r="E24" s="68">
+      <c r="E24" s="67">
         <v>1</v>
       </c>
-      <c r="F24" s="70">
+      <c r="F24" s="38">
         <v>1.8</v>
       </c>
       <c r="G24" s="68" t="s">
@@ -2976,12 +2849,11 @@
     <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2991,341 +2863,343 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="52" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="53" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="52" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="52" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="52" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A1" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="55"/>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="29" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A2" s="44"/>
+      <c r="B2" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="32">
-        <v>3.9300000000000002E-2</v>
-      </c>
-      <c r="C3" s="32">
+      <c r="B3" s="48">
+        <v>0.0393</v>
+      </c>
+      <c r="C3" s="48">
         <v>51.4</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="48">
         <v>0.1</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="48">
         <v>0.03</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="49">
         <v>51.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="32">
-        <v>3.7699999999999997E-2</v>
-      </c>
-      <c r="C4" s="32">
+      <c r="B4" s="48">
+        <v>0.0377</v>
+      </c>
+      <c r="C4" s="48">
         <v>51.4</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="48">
         <v>0.2</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="48">
         <v>0.03</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="49">
         <v>51.63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B5" s="32">
-        <v>3.7699999999999997E-2</v>
-      </c>
-      <c r="C5" s="32">
+      <c r="B5" s="48">
+        <v>0.0377</v>
+      </c>
+      <c r="C5" s="48">
         <v>51.9</v>
       </c>
-      <c r="D5" s="32">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="E5" s="32">
+      <c r="D5" s="48">
+        <v>4.6</v>
+      </c>
+      <c r="E5" s="48">
         <v>0.3</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="49">
         <v>56.8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A6" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="32">
-        <v>3.9300000000000002E-2</v>
-      </c>
-      <c r="C6" s="32">
+      <c r="B6" s="48">
+        <v>0.0393</v>
+      </c>
+      <c r="C6" s="48">
         <v>51.4</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="48">
         <v>0.1</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="48">
         <v>0.03</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="49">
         <v>51.53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A7" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B7" s="32">
-        <v>3.9300000000000002E-2</v>
-      </c>
-      <c r="C7" s="32">
+      <c r="B7" s="48">
+        <v>0.0393</v>
+      </c>
+      <c r="C7" s="48">
         <v>51.4</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="48">
         <v>0.1</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="48">
         <v>0.03</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="49">
         <v>51.53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A8" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="32">
-        <v>6.2899999999999998E-2</v>
-      </c>
-      <c r="C8" s="32">
+      <c r="B8" s="48">
+        <v>0.0629</v>
+      </c>
+      <c r="C8" s="48">
         <v>56.5</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="48">
         <v>0.03</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="48">
         <v>0.03</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="49">
         <v>56.56</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A9" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B9" s="32">
-        <v>1.8100000000000002E-2</v>
-      </c>
-      <c r="C9" s="34">
+      <c r="B9" s="48">
+        <v>0.0181</v>
+      </c>
+      <c r="C9" s="50">
         <v>37</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="48">
         <v>0.03</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="48">
         <v>0.05</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="49">
         <v>37.08</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A10" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="32">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C10" s="34">
+      <c r="B10" s="48">
+        <v>0.004</v>
+      </c>
+      <c r="C10" s="50">
         <v>234</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="48">
         <v>0.03</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="48">
         <v>0.02</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="49">
         <v>234.05</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A11" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="32">
-        <v>3.9E-2</v>
-      </c>
-      <c r="C11" s="32">
+      <c r="B11" s="48">
+        <v>0.039</v>
+      </c>
+      <c r="C11" s="48">
         <v>60.2</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="48">
         <v>0.04</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="48">
         <v>0.03</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="49">
         <v>60.27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A12" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="48">
         <v>51.4</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="48">
         <v>0.1</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="48">
         <v>0.03</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="49">
         <v>51.53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A13" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="32">
-        <v>3.9E-2</v>
-      </c>
-      <c r="C13" s="32">
+      <c r="B13" s="48">
+        <v>0.039</v>
+      </c>
+      <c r="C13" s="48">
         <v>51.4</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="48">
         <v>0.1</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="48">
         <v>0.03</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="49">
         <v>51.53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A14" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="32">
-        <v>3.7699999999999997E-2</v>
-      </c>
-      <c r="C14" s="34">
+      <c r="B14" s="48">
+        <v>0.0377</v>
+      </c>
+      <c r="C14" s="50">
         <v>0</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="48">
         <v>6.4</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="48">
         <v>0.03</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="49">
         <v>6.43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A15" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="32">
-        <v>3.7699999999999997E-2</v>
-      </c>
-      <c r="C15" s="34">
+      <c r="B15" s="48">
+        <v>0.0377</v>
+      </c>
+      <c r="C15" s="50">
         <v>0</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="48">
         <v>6.4</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="48">
         <v>0.03</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="49">
         <v>6.43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A16" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="32">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="C16" s="34">
+      <c r="B16" s="48">
+        <v>0.037</v>
+      </c>
+      <c r="C16" s="50">
         <v>0</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="48">
         <v>6.4</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="48">
         <v>0.03</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="49">
         <v>6.43</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A17" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="32">
-        <v>3.9300000000000002E-2</v>
-      </c>
-      <c r="C17" s="34">
+      <c r="B17" s="48">
+        <v>0.0393</v>
+      </c>
+      <c r="C17" s="50">
         <v>0</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="48">
         <v>0.1</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="48">
         <v>0.03</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="49">
         <v>0.13</v>
       </c>
     </row>
@@ -3339,7 +3213,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3349,127 +3223,130 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="39" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="39" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25" customFormat="1" s="1">
+      <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="15" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="61" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="33" customFormat="1" s="1">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="16" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="17"/>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="29"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33.75" customFormat="1" s="1">
+      <c r="A4" s="30"/>
+      <c r="B4" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="35" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="96" customFormat="1" s="1">
       <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="36" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="12">
         <v>13.9</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="37">
         <v>0</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="37">
         <v>0</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="38">
         <v>13.9</v>
       </c>
       <c r="G5" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="36" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="12">
         <v>3.5</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="37">
         <v>0</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="37">
         <v>0</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="38">
         <v>3.5</v>
       </c>
       <c r="G6" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="57.75" customFormat="1" s="1">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="36" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="12">
-        <v>69.599999999999994</v>
+        <v>69.6</v>
       </c>
       <c r="D7" s="12">
         <v>0.08</v>
@@ -3477,21 +3354,21 @@
       <c r="E7" s="12">
         <v>0.2</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="38">
         <v>69.88</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="25">
+      <c r="C8" s="37">
         <v>61</v>
       </c>
       <c r="D8" s="12">
@@ -3500,22 +3377,22 @@
       <c r="E8" s="12">
         <v>0.2</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="38">
         <v>61.28</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="70.5" customFormat="1" s="1">
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="12">
-        <v>67.400000000000006</v>
+        <v>67.4</v>
       </c>
       <c r="D9" s="12">
         <v>0.2</v>
@@ -3523,21 +3400,21 @@
       <c r="E9" s="12">
         <v>0.2</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="38">
         <v>67.8</v>
       </c>
       <c r="G9" s="5">
         <v>17.2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="25">
+      <c r="C10" s="37">
         <v>67</v>
       </c>
       <c r="D10" s="12">
@@ -3546,22 +3423,22 @@
       <c r="E10" s="12">
         <v>0.2</v>
       </c>
-      <c r="F10" s="26">
-        <v>67.400000000000006</v>
+      <c r="F10" s="38">
+        <v>67.4</v>
       </c>
       <c r="G10" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="57.75" customFormat="1" s="1">
       <c r="A11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="36" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="12">
-        <v>68.900000000000006</v>
+        <v>68.9</v>
       </c>
       <c r="D11" s="12">
         <v>0.01</v>
@@ -3569,22 +3446,22 @@
       <c r="E11" s="12">
         <v>0.2</v>
       </c>
-      <c r="F11" s="26">
+      <c r="F11" s="38">
         <v>69.11</v>
       </c>
       <c r="G11" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="36" t="s">
         <v>61</v>
       </c>
       <c r="C12" s="12">
-        <v>69.599999999999994</v>
+        <v>69.6</v>
       </c>
       <c r="D12" s="12">
         <v>0.02</v>
@@ -3592,18 +3469,18 @@
       <c r="E12" s="12">
         <v>0.2</v>
       </c>
-      <c r="F12" s="26">
-        <v>69.819999999999993</v>
+      <c r="F12" s="38">
+        <v>69.82</v>
       </c>
       <c r="G12" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="36" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="12">
@@ -3615,22 +3492,22 @@
       <c r="E13" s="12">
         <v>0.2</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="38">
         <v>69.73</v>
       </c>
       <c r="G13" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A14" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="36" t="s">
         <v>65</v>
       </c>
       <c r="C14" s="12">
-        <v>69.900000000000006</v>
+        <v>69.9</v>
       </c>
       <c r="D14" s="12">
         <v>0.1</v>
@@ -3638,22 +3515,22 @@
       <c r="E14" s="12">
         <v>0.2</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="38">
         <v>70.2</v>
       </c>
       <c r="G14" s="5">
         <v>17.3</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="36" t="s">
         <v>67</v>
       </c>
       <c r="C15" s="12">
-        <v>73.599999999999994</v>
+        <v>73.6</v>
       </c>
       <c r="D15" s="12">
         <v>0.04</v>
@@ -3661,18 +3538,18 @@
       <c r="E15" s="12">
         <v>0.2</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="38">
         <v>73.84</v>
       </c>
       <c r="G15" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="36" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="12">
@@ -3684,18 +3561,18 @@
       <c r="E16" s="12">
         <v>0.2</v>
       </c>
-      <c r="F16" s="26">
-        <v>69.930000000000007</v>
+      <c r="F16" s="38">
+        <v>69.93</v>
       </c>
       <c r="G16" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="57.75" customFormat="1" s="1">
       <c r="A17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="36" t="s">
         <v>69</v>
       </c>
       <c r="C17" s="12">
@@ -3707,18 +3584,18 @@
       <c r="E17" s="12">
         <v>0.2</v>
       </c>
-      <c r="F17" s="26">
-        <v>69.930000000000007</v>
+      <c r="F17" s="38">
+        <v>69.93</v>
       </c>
       <c r="G17" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="45" customFormat="1" s="1">
       <c r="A18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="36" t="s">
         <v>72</v>
       </c>
       <c r="C18" s="12">
@@ -3730,18 +3607,18 @@
       <c r="E18" s="12">
         <v>0.2</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="38">
         <v>60.6</v>
       </c>
       <c r="G18" s="5">
         <v>20.2</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A19" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="36" t="s">
         <v>74</v>
       </c>
       <c r="C19" s="12">
@@ -3753,18 +3630,18 @@
       <c r="E19" s="12">
         <v>0.01</v>
       </c>
-      <c r="F19" s="26">
-        <v>69.819999999999993</v>
+      <c r="F19" s="38">
+        <v>69.82</v>
       </c>
       <c r="G19" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A20" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="36" t="s">
         <v>76</v>
       </c>
       <c r="C20" s="12">
@@ -3776,18 +3653,18 @@
       <c r="E20" s="12">
         <v>0.2</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="38">
         <v>92.88</v>
       </c>
       <c r="G20" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="36" t="s">
         <v>78</v>
       </c>
       <c r="C21" s="12">
@@ -3799,18 +3676,18 @@
       <c r="E21" s="12">
         <v>0.03</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="38">
         <v>54.76</v>
       </c>
       <c r="G21" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A22" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="36" t="s">
         <v>76</v>
       </c>
       <c r="C22" s="12">
@@ -3822,18 +3699,18 @@
       <c r="E22" s="12">
         <v>0.2</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="38">
         <v>92.88</v>
       </c>
       <c r="G22" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A23" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="36" t="s">
         <v>69</v>
       </c>
       <c r="C23" s="12">
@@ -3845,21 +3722,21 @@
       <c r="E23" s="12">
         <v>0.1</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="38">
         <v>69.92</v>
       </c>
       <c r="G23" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="37">
         <v>0</v>
       </c>
       <c r="D24" s="12">
@@ -3868,21 +3745,21 @@
       <c r="E24" s="12">
         <v>0.2</v>
       </c>
-      <c r="F24" s="26">
-        <v>0.28000000000000003</v>
+      <c r="F24" s="38">
+        <v>0.28</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A25" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="37">
         <v>0</v>
       </c>
       <c r="D25" s="12">
@@ -3891,21 +3768,21 @@
       <c r="E25" s="12">
         <v>0.2</v>
       </c>
-      <c r="F25" s="26">
-        <v>0.28000000000000003</v>
+      <c r="F25" s="38">
+        <v>0.28</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A26" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="37">
         <v>0</v>
       </c>
       <c r="D26" s="12">
@@ -3914,8 +3791,8 @@
       <c r="E26" s="12">
         <v>0.2</v>
       </c>
-      <c r="F26" s="26">
-        <v>0.28000000000000003</v>
+      <c r="F26" s="38">
+        <v>0.28</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>51</v>
@@ -3934,7 +3811,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3944,12 +3821,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="27.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A1" s="8" t="s">
         <v>19</v>
       </c>
@@ -3960,7 +3837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -3971,7 +3848,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
@@ -3982,7 +3859,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A4" s="4" t="s">
         <v>24</v>
       </c>
@@ -3993,7 +3870,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -4004,7 +3881,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -4012,10 +3889,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="5">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -4026,7 +3903,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
@@ -4037,7 +3914,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A9" s="4" t="s">
         <v>29</v>
       </c>
@@ -4045,21 +3922,21 @@
         <v>3.3</v>
       </c>
       <c r="C9" s="5">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="12">
         <v>0.42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A11" s="13" t="s">
         <v>31</v>
       </c>
@@ -4067,10 +3944,10 @@
         <v>1.6</v>
       </c>
       <c r="C11" s="14">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
@@ -4078,10 +3955,10 @@
         <v>1.3</v>
       </c>
       <c r="C12" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A13" s="4" t="s">
         <v>33</v>
       </c>
@@ -4089,7 +3966,7 @@
         <v>0.2</v>
       </c>
       <c r="C13" s="5">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
     </row>
   </sheetData>
@@ -4098,7 +3975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4108,11 +3985,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="21.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -4120,15 +3997,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
@@ -4136,7 +4013,7 @@
         <v>0.1229</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -4144,15 +4021,15 @@
         <v>0.3276</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="5">
-        <v>8.1900000000000001E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.0819</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -4166,7 +4043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4176,32 +4053,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="15.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="61.5" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5">
-        <v>4.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.046</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="32.25" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5">
-        <v>2.8000000000000001E-2</v>
+        <v>0.028</v>
       </c>
     </row>
   </sheetData>
@@ -4210,7 +4087,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4220,53 +4097,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="6" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="19.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5">
         <v>0.879</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A3" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>2.931</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="5">
         <v>1.649</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>5.36</v>

</xml_diff>

<commit_message>
Added Natural Gas table
</commit_message>
<xml_diff>
--- a/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
+++ b/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
@@ -8,26 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marsh\Documents\Infosys\EcoTrack\EcoTrackFront-End\ecotrack-backend\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD27481-2225-4C70-BC69-6E1F9BD9B4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C98795-B343-46C2-977C-8C7EC8469D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity" sheetId="1" r:id="rId1"/>
     <sheet name="Solid Fuel" sheetId="2" r:id="rId2"/>
     <sheet name="Gaseous Fuel" sheetId="3" r:id="rId3"/>
-    <sheet name="Liquid Fuel" sheetId="4" r:id="rId4"/>
-    <sheet name="Solid Waste" sheetId="5" r:id="rId5"/>
-    <sheet name="Wastewater Treatment" sheetId="6" r:id="rId6"/>
-    <sheet name="Waste Incineration" sheetId="7" r:id="rId7"/>
-    <sheet name="Biological Treatment" sheetId="8" r:id="rId8"/>
+    <sheet name="Natural Gas Data" sheetId="9" r:id="rId4"/>
+    <sheet name="Liquid Fuel" sheetId="4" r:id="rId5"/>
+    <sheet name="Solid Waste" sheetId="5" r:id="rId6"/>
+    <sheet name="Wastewater Treatment" sheetId="6" r:id="rId7"/>
+    <sheet name="Waste Incineration" sheetId="7" r:id="rId8"/>
+    <sheet name="Biological Treatment" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="157">
   <si>
     <t xml:space="preserve">Waste treatment type  </t>
   </si>
@@ -1067,13 +1068,56 @@
   </si>
   <si>
     <t>Municipal Solid Waste</t>
+  </si>
+  <si>
+    <t>State or territory</t>
+  </si>
+  <si>
+    <r>
+      <t>Scope 3 Emission Factors for Natural Gas (kg CO</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-e /GJ)</t>
+    </r>
+  </si>
+  <si>
+    <t>Metro</t>
+  </si>
+  <si>
+    <t>Non-metro</t>
+  </si>
+  <si>
+    <t>New South Wales and ACT</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1179,8 +1223,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1202,8 +1255,14 @@
         <fgColor rgb="FFE2F1EE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF083A42"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1572,11 +1631,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF8EC8BF"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF8EC8BF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF8EC8BF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1716,6 +1788,18 @@
     <xf numFmtId="3" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1728,18 +1812,6 @@
     <xf numFmtId="3" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1826,6 +1898,27 @@
     </xf>
     <xf numFmtId="4" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2148,20 +2241,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="49" t="s">
+      <c r="C1" s="54"/>
+      <c r="D1" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="50"/>
+      <c r="E1" s="54"/>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
+      <c r="A2" s="52"/>
       <c r="B2" s="42" t="s">
         <v>129</v>
       </c>
@@ -2247,16 +2340,16 @@
       <c r="A7" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="B7" s="51">
+      <c r="B7" s="47">
         <v>0.51</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="49">
         <v>164</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="47">
         <v>0.04</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="49">
         <v>12</v>
       </c>
     </row>
@@ -2264,10 +2357,10 @@
       <c r="A8" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B8" s="52"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="54"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="50"/>
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -2290,16 +2383,16 @@
       <c r="A10" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="B10" s="51">
+      <c r="B10" s="47">
         <v>0.54</v>
       </c>
-      <c r="C10" s="53">
+      <c r="C10" s="49">
         <v>152</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="47">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E10" s="53">
+      <c r="E10" s="49">
         <v>19</v>
       </c>
     </row>
@@ -2307,10 +2400,10 @@
       <c r="A11" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="54"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="48"/>
+      <c r="E11" s="50"/>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -3273,6 +3366,121 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA22915-536E-41BF-8720-9566AA07CB47}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="87" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="90"/>
+    </row>
+    <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="88"/>
+      <c r="B2" s="84" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="85" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="86">
+        <v>13.1</v>
+      </c>
+      <c r="C3" s="86">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="85" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="86">
+        <v>4</v>
+      </c>
+      <c r="C4" s="86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="85" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="86">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C5" s="86">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="85" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="86">
+        <v>10.7</v>
+      </c>
+      <c r="C6" s="86">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="85" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="86">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C7" s="86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="85" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="86" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="86" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="85" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="86" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="86" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -3292,10 +3500,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="51" t="s">
         <v>29</v>
       </c>
       <c r="C1" s="77" t="s">
@@ -3869,7 +4077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -4035,7 +4243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -4105,7 +4313,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -4175,14 +4383,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Separated kL and t in spreadsheet
</commit_message>
<xml_diff>
--- a/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
+++ b/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
@@ -8,27 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marsh\Documents\Infosys\EcoTrack\EcoTrackFront-End\ecotrack-backend\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C98795-B343-46C2-977C-8C7EC8469D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B733FEA1-C341-4116-88E3-63DE83308B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity" sheetId="1" r:id="rId1"/>
     <sheet name="Solid Fuel" sheetId="2" r:id="rId2"/>
     <sheet name="Gaseous Fuel" sheetId="3" r:id="rId3"/>
     <sheet name="Natural Gas Data" sheetId="9" r:id="rId4"/>
-    <sheet name="Liquid Fuel" sheetId="4" r:id="rId5"/>
-    <sheet name="Solid Waste" sheetId="5" r:id="rId6"/>
-    <sheet name="Wastewater Treatment" sheetId="6" r:id="rId7"/>
-    <sheet name="Waste Incineration" sheetId="7" r:id="rId8"/>
-    <sheet name="Biological Treatment" sheetId="8" r:id="rId9"/>
+    <sheet name="Liquid Fuel kL" sheetId="4" r:id="rId5"/>
+    <sheet name="Liquid Fuel t" sheetId="10" r:id="rId6"/>
+    <sheet name="Solid Waste" sheetId="5" r:id="rId7"/>
+    <sheet name="Wastewater Treatment" sheetId="6" r:id="rId8"/>
+    <sheet name="Waste Incineration" sheetId="7" r:id="rId9"/>
+    <sheet name="Biological Treatment" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="145">
   <si>
     <t xml:space="preserve">Waste treatment type  </t>
   </si>
@@ -274,9 +275,6 @@
     <t>Emission factor</t>
   </si>
   <si>
-    <t>(GJ per unit of fuel)</t>
-  </si>
-  <si>
     <r>
       <t>CO</t>
     </r>
@@ -369,22 +367,6 @@
     <t>Petroleum based oils (other than petroleum based oil used as fuel), e.g. lubricants</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">38.8 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Petroleum based greases</t>
   </si>
   <si>
@@ -406,193 +388,33 @@
     <t>Automotive gasoline/petrol (other than for use as fuel in an aircraft)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">34.2 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Aviation gasoline</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">33.1 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Kerosene (other than for use as fuel in an aircraft)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">37.5 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">36.8 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Heating oil</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">37.3 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Diesel oil</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">38.6 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Fuel oil</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">39.7 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Liquefied aromatic hydrocarbons</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">34.4 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Solvents: mineral turpentine or white spirits</t>
   </si>
   <si>
     <t>Liquefied petroleum gas (LPG)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">25.7 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Naphtha</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">31.4 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Petroleum coke</t>
   </si>
   <si>
@@ -614,39 +436,7 @@
     <t>Biodiesel</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">34.6 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
-  </si>
-  <si>
     <t>Ethanol for use as a fuel in an internal combustion engine</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">23.4 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GJ/kL</t>
-    </r>
   </si>
   <si>
     <t>Biofuels other than those mentioned in the items above</t>
@@ -1112,12 +902,18 @@
   <si>
     <t>C</t>
   </si>
+  <si>
+    <t>(GJ per kL)</t>
+  </si>
+  <si>
+    <t>(GJ per t)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1181,14 +977,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1788,6 +1576,15 @@
     <xf numFmtId="3" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1872,6 +1669,18 @@
     <xf numFmtId="4" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1898,27 +1707,6 @@
     </xf>
     <xf numFmtId="4" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2231,46 +2019,46 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="53" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="53" t="s">
-        <v>128</v>
-      </c>
-      <c r="E1" s="54"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="57"/>
+      <c r="D1" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="57"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="55"/>
       <c r="B2" s="42" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B3" s="5">
         <v>0.73</v>
@@ -2285,9 +2073,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B4" s="5">
         <v>0.85</v>
@@ -2302,9 +2090,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B5" s="5">
         <v>0.73</v>
@@ -2319,9 +2107,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B6" s="5">
         <v>0.25</v>
@@ -2336,35 +2124,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="47">
+        <v>121</v>
+      </c>
+      <c r="B7" s="50">
         <v>0.51</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="52">
         <v>164</v>
       </c>
-      <c r="D7" s="47">
+      <c r="D7" s="50">
         <v>0.04</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="52">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="50"/>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="B8" s="51"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="53"/>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B9" s="5">
         <v>0.17</v>
@@ -2379,35 +2167,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" s="47">
+        <v>124</v>
+      </c>
+      <c r="B10" s="50">
         <v>0.54</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="52">
         <v>152</v>
       </c>
-      <c r="D10" s="47">
+      <c r="D10" s="50">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="52">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="48"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="50"/>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="53"/>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B12" s="5">
         <v>0.57999999999999996</v>
@@ -2416,15 +2204,15 @@
         <v>160</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="45" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="B13" s="26">
         <v>0.68</v>
@@ -2457,6 +2245,52 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
@@ -2468,66 +2302,66 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
-        <v>98</v>
-      </c>
-      <c r="B1" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="68" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="69"/>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="59"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="72"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="60"/>
       <c r="B3" s="22" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="38" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B4" s="39">
         <v>27</v>
@@ -2548,9 +2382,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="38" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B5" s="39">
         <v>21</v>
@@ -2571,9 +2405,9 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B6" s="39">
         <v>29</v>
@@ -2591,12 +2425,12 @@
         <v>90.24</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="38" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B7" s="40">
         <v>10.199999999999999</v>
@@ -2617,9 +2451,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B8" s="39">
         <v>30</v>
@@ -2640,9 +2474,9 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="38" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B9" s="40">
         <v>22.1</v>
@@ -2660,12 +2494,12 @@
         <v>95.38</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="38" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B10" s="39">
         <v>27</v>
@@ -2683,12 +2517,12 @@
         <v>107.23</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="38" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B11" s="40">
         <v>37.5</v>
@@ -2706,10 +2540,10 @@
         <v>82.03</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="38"/>
       <c r="B12" s="40"/>
       <c r="C12" s="39"/>
@@ -2718,9 +2552,9 @@
       <c r="F12" s="41"/>
       <c r="G12" s="40"/>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="38" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B13" s="40">
         <v>22.1</v>
@@ -2738,12 +2572,12 @@
         <v>95.28</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="38" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B14" s="40">
         <v>26.3</v>
@@ -2761,12 +2595,12 @@
         <v>81.83</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="38" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="B15" s="39">
         <v>32</v>
@@ -2784,12 +2618,12 @@
         <v>63.03</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="38" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B16" s="40">
         <v>27.1</v>
@@ -2807,12 +2641,12 @@
         <v>56.13</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="38" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B17" s="40">
         <v>10.5</v>
@@ -2830,12 +2664,12 @@
         <v>88.9</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="38" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B18" s="40">
         <v>16.2</v>
@@ -2853,12 +2687,12 @@
         <v>1.2</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="38" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B19" s="40">
         <v>10.4</v>
@@ -2876,12 +2710,12 @@
         <v>1.2</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="38" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B20" s="40">
         <v>12.4</v>
@@ -2899,12 +2733,12 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="38" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B21" s="40">
         <v>9.6</v>
@@ -2922,12 +2756,12 @@
         <v>1.4</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="38" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B22" s="40">
         <v>12.2</v>
@@ -2945,12 +2779,12 @@
         <v>1.8</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="38" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B23" s="40">
         <v>31.1</v>
@@ -2968,12 +2802,12 @@
         <v>6.3</v>
       </c>
       <c r="G23" s="40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B24" s="40">
         <v>12.2</v>
@@ -2991,7 +2825,7 @@
         <v>1.8</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -3016,49 +2850,49 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5546875" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="74"/>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71"/>
+        <v>65</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="77"/>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="74"/>
       <c r="B2" s="29" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C2" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="E2" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="F2" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B3" s="32">
         <v>3.9300000000000002E-2</v>
@@ -3076,9 +2910,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B4" s="32">
         <v>3.7699999999999997E-2</v>
@@ -3096,9 +2930,9 @@
         <v>51.63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B5" s="32">
         <v>3.7699999999999997E-2</v>
@@ -3116,9 +2950,9 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B6" s="32">
         <v>3.9300000000000002E-2</v>
@@ -3136,9 +2970,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B7" s="32">
         <v>3.9300000000000002E-2</v>
@@ -3156,9 +2990,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B8" s="32">
         <v>6.2899999999999998E-2</v>
@@ -3176,9 +3010,9 @@
         <v>56.56</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B9" s="32">
         <v>1.8100000000000002E-2</v>
@@ -3196,9 +3030,9 @@
         <v>37.08</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B10" s="32">
         <v>4.0000000000000001E-3</v>
@@ -3216,9 +3050,9 @@
         <v>234.05</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B11" s="32">
         <v>3.9E-2</v>
@@ -3236,12 +3070,12 @@
         <v>60.27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C12" s="32">
         <v>51.4</v>
@@ -3256,9 +3090,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B13" s="32">
         <v>3.9E-2</v>
@@ -3276,9 +3110,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B14" s="32">
         <v>3.7699999999999997E-2</v>
@@ -3296,9 +3130,9 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B15" s="32">
         <v>3.7699999999999997E-2</v>
@@ -3316,9 +3150,9 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B16" s="32">
         <v>3.6999999999999998E-2</v>
@@ -3336,9 +3170,9 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B17" s="32">
         <v>3.9300000000000002E-2</v>
@@ -3369,105 +3203,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA22915-536E-41BF-8720-9566AA07CB47}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="87" t="s">
-        <v>151</v>
-      </c>
-      <c r="B1" s="89" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="90"/>
-    </row>
-    <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="88"/>
-      <c r="B2" s="84" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="84" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="85" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3" s="86">
+    <row r="1" spans="1:3" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="78" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="81"/>
+    </row>
+    <row r="2" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="79"/>
+      <c r="B2" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="48" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="49">
         <v>13.1</v>
       </c>
-      <c r="C3" s="86">
+      <c r="C3" s="49">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="85" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="86">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="48" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="49">
         <v>4</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="85" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="86">
+    <row r="5" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="49">
         <v>8.8000000000000007</v>
       </c>
-      <c r="C5" s="86">
+      <c r="C5" s="49">
         <v>7.9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="85" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="86">
+    <row r="6" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="49">
         <v>10.7</v>
       </c>
-      <c r="C6" s="86">
+      <c r="C6" s="49">
         <v>10.6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="85" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="86">
+    <row r="7" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="49">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C7" s="86">
+      <c r="C7" s="49">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="85" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="86" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" s="86" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="85" t="s">
-        <v>138</v>
-      </c>
-      <c r="B9" s="86" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="86" t="s">
-        <v>156</v>
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3487,84 +3321,84 @@
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="63"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="66"/>
       <c r="G1" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75"/>
-      <c r="B2" s="75"/>
-      <c r="C2" s="78" t="s">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="80"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
-      <c r="B3" s="76"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="83"/>
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="83"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="90"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="D4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="G4" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="23" t="s">
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="24" t="s">
-        <v>41</v>
+      <c r="B5" s="24">
+        <v>38.799999999999997</v>
       </c>
       <c r="C5" s="12">
         <v>13.9</v>
@@ -3582,12 +3416,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B6" s="24">
+        <v>38.799999999999997</v>
       </c>
       <c r="C6" s="12">
         <v>3.5</v>
@@ -3605,314 +3439,314 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>44</v>
+        <v>46</v>
+      </c>
+      <c r="B7" s="24">
+        <v>34.200000000000003</v>
       </c>
       <c r="C7" s="12">
-        <v>69.599999999999994</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="D7" s="12">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E7" s="12">
         <v>0.2</v>
       </c>
       <c r="F7" s="26">
-        <v>69.88</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67.8</v>
+      </c>
+      <c r="G7" s="5">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="24" t="s">
         <v>47</v>
       </c>
+      <c r="B8" s="24">
+        <v>33.1</v>
+      </c>
       <c r="C8" s="25">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D8" s="12">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="E8" s="12">
         <v>0.2</v>
       </c>
       <c r="F8" s="26">
-        <v>61.28</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="G8" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>49</v>
+      <c r="B9" s="24">
+        <v>37.5</v>
       </c>
       <c r="C9" s="12">
-        <v>67.400000000000006</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="D9" s="12">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="E9" s="12">
         <v>0.2</v>
       </c>
       <c r="F9" s="26">
-        <v>67.8</v>
-      </c>
-      <c r="G9" s="5">
-        <v>17.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69.11</v>
+      </c>
+      <c r="G9" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="25">
-        <v>67</v>
+        <v>130</v>
+      </c>
+      <c r="B10" s="24">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="C10" s="12">
+        <v>69.599999999999994</v>
       </c>
       <c r="D10" s="12">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="E10" s="12">
         <v>0.2</v>
       </c>
       <c r="F10" s="26">
-        <v>67.400000000000006</v>
+        <v>69.819999999999993</v>
       </c>
       <c r="G10" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="B11" s="24">
+        <v>37.299999999999997</v>
       </c>
       <c r="C11" s="12">
-        <v>68.900000000000006</v>
+        <v>69.5</v>
       </c>
       <c r="D11" s="12">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E11" s="12">
         <v>0.2</v>
       </c>
       <c r="F11" s="26">
-        <v>69.11</v>
+        <v>69.73</v>
       </c>
       <c r="G11" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B12" s="24" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="B12" s="24">
+        <v>38.6</v>
       </c>
       <c r="C12" s="12">
-        <v>69.599999999999994</v>
+        <v>69.900000000000006</v>
       </c>
       <c r="D12" s="12">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="E12" s="12">
         <v>0.2</v>
       </c>
       <c r="F12" s="26">
-        <v>69.819999999999993</v>
-      </c>
-      <c r="G12" s="11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70.2</v>
+      </c>
+      <c r="G12" s="5">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="B13" s="24">
+        <v>39.700000000000003</v>
       </c>
       <c r="C13" s="12">
-        <v>69.5</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="D13" s="12">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E13" s="12">
         <v>0.2</v>
       </c>
       <c r="F13" s="26">
-        <v>69.73</v>
+        <v>73.84</v>
       </c>
       <c r="G13" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="B14" s="24">
+        <v>34.4</v>
       </c>
       <c r="C14" s="12">
-        <v>69.900000000000006</v>
+        <v>69.7</v>
       </c>
       <c r="D14" s="12">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="E14" s="12">
         <v>0.2</v>
       </c>
       <c r="F14" s="26">
-        <v>70.2</v>
-      </c>
-      <c r="G14" s="5">
-        <v>17.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69.930000000000007</v>
+      </c>
+      <c r="G14" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>60</v>
+        <v>53</v>
+      </c>
+      <c r="B15" s="24">
+        <v>34.4</v>
       </c>
       <c r="C15" s="12">
-        <v>73.599999999999994</v>
+        <v>69.7</v>
       </c>
       <c r="D15" s="12">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="E15" s="12">
         <v>0.2</v>
       </c>
       <c r="F15" s="26">
-        <v>73.84</v>
+        <v>69.930000000000007</v>
       </c>
       <c r="G15" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="B16" s="24">
+        <v>25.7</v>
       </c>
       <c r="C16" s="12">
-        <v>69.7</v>
+        <v>60.2</v>
       </c>
       <c r="D16" s="12">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
       <c r="E16" s="12">
         <v>0.2</v>
       </c>
       <c r="F16" s="26">
-        <v>69.930000000000007</v>
-      </c>
-      <c r="G16" s="11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60.6</v>
+      </c>
+      <c r="G16" s="5">
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="B17" s="24">
+        <v>31.4</v>
       </c>
       <c r="C17" s="12">
-        <v>69.7</v>
+        <v>69.8</v>
       </c>
       <c r="D17" s="12">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E17" s="12">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="F17" s="26">
-        <v>69.930000000000007</v>
+        <v>69.819999999999993</v>
       </c>
       <c r="G17" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="B18" s="24">
+        <v>34.4</v>
       </c>
       <c r="C18" s="12">
-        <v>60.2</v>
+        <v>69.8</v>
       </c>
       <c r="D18" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="E18" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="26">
+        <v>69.92</v>
+      </c>
+      <c r="G18" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="24">
+        <v>34.6</v>
+      </c>
+      <c r="C19" s="25">
+        <v>0</v>
+      </c>
+      <c r="D19" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="E19" s="12">
         <v>0.2</v>
       </c>
-      <c r="E18" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="F18" s="26">
-        <v>60.6</v>
-      </c>
-      <c r="G18" s="5">
-        <v>20.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="12">
-        <v>69.8</v>
-      </c>
-      <c r="D19" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="E19" s="12">
-        <v>0.01</v>
-      </c>
       <c r="F19" s="26">
-        <v>69.819999999999993</v>
-      </c>
-      <c r="G19" s="11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="12">
-        <v>92.6</v>
+        <v>63</v>
+      </c>
+      <c r="B20" s="24">
+        <v>23.4</v>
+      </c>
+      <c r="C20" s="25">
+        <v>0</v>
       </c>
       <c r="D20" s="12">
         <v>0.08</v>
@@ -3921,150 +3755,40 @@
         <v>0.2</v>
       </c>
       <c r="F20" s="26">
-        <v>92.88</v>
-      </c>
-      <c r="G20" s="11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="12">
-        <v>54.7</v>
+        <v>64</v>
+      </c>
+      <c r="B21" s="24">
+        <v>23.4</v>
+      </c>
+      <c r="C21" s="25">
+        <v>0</v>
       </c>
       <c r="D21" s="12">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E21" s="12">
-        <v>0.03</v>
+        <v>0.2</v>
       </c>
       <c r="F21" s="26">
-        <v>54.76</v>
-      </c>
-      <c r="G21" s="11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="12">
-        <v>92.6</v>
-      </c>
-      <c r="D22" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="E22" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="F22" s="26">
-        <v>92.88</v>
-      </c>
-      <c r="G22" s="11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="12">
-        <v>69.8</v>
-      </c>
-      <c r="D23" s="12">
-        <v>0.02</v>
-      </c>
-      <c r="E23" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="F23" s="26">
-        <v>69.92</v>
-      </c>
-      <c r="G23" s="11">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="25">
-        <v>0</v>
-      </c>
-      <c r="D24" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="E24" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="F24" s="26">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G24" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" s="25">
-        <v>0</v>
-      </c>
-      <c r="D25" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="E25" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="F25" s="26">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="25">
-        <v>0</v>
-      </c>
-      <c r="D26" s="12">
-        <v>0.08</v>
-      </c>
-      <c r="E26" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="F26" s="26">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>45</v>
-      </c>
-    </row>
+      <c r="G21" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A3"/>
@@ -4078,6 +3802,203 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEC68CE-6DD4-4E91-98E5-118BA2896909}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="83"/>
+      <c r="B3" s="83"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="17"/>
+    </row>
+    <row r="4" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="12">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="D5" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="26">
+        <v>69.88</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="25">
+        <v>61</v>
+      </c>
+      <c r="D6" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="E6" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="26">
+        <v>61.28</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="12">
+        <v>92.6</v>
+      </c>
+      <c r="D7" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="E7" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="26">
+        <v>92.88</v>
+      </c>
+      <c r="G7" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="12">
+        <v>54.7</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="E8" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="F8" s="26">
+        <v>54.76</v>
+      </c>
+      <c r="G8" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="12">
+        <v>92.6</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0.08</v>
+      </c>
+      <c r="E9" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="26">
+        <v>92.88</v>
+      </c>
+      <c r="G9" s="11">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -4088,14 +4009,14 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5546875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
@@ -4106,7 +4027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -4117,7 +4038,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -4128,7 +4049,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -4139,7 +4060,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -4150,7 +4071,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -4161,7 +4082,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -4172,7 +4093,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -4183,7 +4104,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -4194,7 +4115,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -4205,7 +4126,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>25</v>
       </c>
@@ -4216,7 +4137,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -4227,7 +4148,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -4243,7 +4164,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -4254,13 +4175,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -4268,7 +4189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -4276,7 +4197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -4284,7 +4205,7 @@
         <v>0.1229</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -4292,7 +4213,7 @@
         <v>0.3276</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -4300,7 +4221,7 @@
         <v>8.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -4313,7 +4234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -4324,104 +4245,58 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B2" s="5">
         <v>0.879</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B4" s="5">
         <v>2.931</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B5" s="5">
         <v>1.649</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="B6" s="5">
         <v>5.36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5">
-        <v>4.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2.8000000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Getting rid of string units
</commit_message>
<xml_diff>
--- a/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
+++ b/ecotrack-backend/Documentation/Emission_Source_Parameters_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marsh\Documents\Infosys\EcoTrack\EcoTrackFront-End\ecotrack-backend\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B733FEA1-C341-4116-88E3-63DE83308B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDACFFA3-124C-429D-9E58-11A2B34B614E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Electricity" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="141">
   <si>
     <t xml:space="preserve">Waste treatment type  </t>
   </si>
@@ -373,18 +373,12 @@
     <t>Crude oil including crude oil condensates</t>
   </si>
   <si>
-    <t>45.3 GJ/t</t>
-  </si>
-  <si>
     <t>NE</t>
   </si>
   <si>
     <t>Other natural gas liquids</t>
   </si>
   <si>
-    <t>46.5 GJ/t</t>
-  </si>
-  <si>
     <t>Automotive gasoline/petrol (other than for use as fuel in an aircraft)</t>
   </si>
   <si>
@@ -418,13 +412,7 @@
     <t>Petroleum coke</t>
   </si>
   <si>
-    <t>34.2 GJ/t</t>
-  </si>
-  <si>
     <t>Refinery gas and liquids</t>
-  </si>
-  <si>
-    <t>42.9 GJ/t</t>
   </si>
   <si>
     <t>Refinery coke</t>
@@ -2019,46 +2007,46 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B1" s="56" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C1" s="57"/>
       <c r="D1" s="56" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E1" s="57"/>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55"/>
       <c r="B2" s="42" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B3" s="5">
         <v>0.73</v>
@@ -2073,9 +2061,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B4" s="5">
         <v>0.85</v>
@@ -2090,9 +2078,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B5" s="5">
         <v>0.73</v>
@@ -2107,9 +2095,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B6" s="5">
         <v>0.25</v>
@@ -2124,9 +2112,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B7" s="50">
         <v>0.51</v>
@@ -2141,18 +2129,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B8" s="51"/>
       <c r="C8" s="53"/>
       <c r="D8" s="51"/>
       <c r="E8" s="53"/>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B9" s="5">
         <v>0.17</v>
@@ -2167,9 +2155,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B10" s="50">
         <v>0.54</v>
@@ -2184,18 +2172,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B11" s="51"/>
       <c r="C11" s="53"/>
       <c r="D11" s="51"/>
       <c r="E11" s="53"/>
     </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B12" s="5">
         <v>0.57999999999999996</v>
@@ -2204,15 +2192,15 @@
         <v>160</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B13" s="26">
         <v>0.68</v>
@@ -2256,13 +2244,13 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2270,7 +2258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -2278,7 +2266,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2302,34 +2290,34 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="58" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B1" s="61" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C1" s="63" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D1" s="64"/>
       <c r="E1" s="65"/>
       <c r="F1" s="66"/>
       <c r="G1" s="71" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59"/>
       <c r="B2" s="62"/>
       <c r="C2" s="67"/>
@@ -2338,30 +2326,30 @@
       <c r="F2" s="70"/>
       <c r="G2" s="72"/>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="60"/>
       <c r="B3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="G3" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="22" t="s">
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
         <v>90</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="38" t="s">
-        <v>94</v>
       </c>
       <c r="B4" s="39">
         <v>27</v>
@@ -2382,9 +2370,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B5" s="39">
         <v>21</v>
@@ -2405,9 +2393,9 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B6" s="39">
         <v>29</v>
@@ -2425,12 +2413,12 @@
         <v>90.24</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B7" s="40">
         <v>10.199999999999999</v>
@@ -2451,9 +2439,9 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B8" s="39">
         <v>30</v>
@@ -2474,9 +2462,9 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B9" s="40">
         <v>22.1</v>
@@ -2494,12 +2482,12 @@
         <v>95.38</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="38" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B10" s="39">
         <v>27</v>
@@ -2517,12 +2505,12 @@
         <v>107.23</v>
       </c>
       <c r="G10" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B11" s="40">
         <v>37.5</v>
@@ -2540,10 +2528,10 @@
         <v>82.03</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="38"/>
       <c r="B12" s="40"/>
       <c r="C12" s="39"/>
@@ -2552,9 +2540,9 @@
       <c r="F12" s="41"/>
       <c r="G12" s="40"/>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B13" s="40">
         <v>22.1</v>
@@ -2572,12 +2560,12 @@
         <v>95.28</v>
       </c>
       <c r="G13" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B14" s="40">
         <v>26.3</v>
@@ -2595,12 +2583,12 @@
         <v>81.83</v>
       </c>
       <c r="G14" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B15" s="39">
         <v>32</v>
@@ -2618,12 +2606,12 @@
         <v>63.03</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="38" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B16" s="40">
         <v>27.1</v>
@@ -2641,12 +2629,12 @@
         <v>56.13</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B17" s="40">
         <v>10.5</v>
@@ -2664,12 +2652,12 @@
         <v>88.9</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B18" s="40">
         <v>16.2</v>
@@ -2687,12 +2675,12 @@
         <v>1.2</v>
       </c>
       <c r="G18" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B19" s="40">
         <v>10.4</v>
@@ -2710,12 +2698,12 @@
         <v>1.2</v>
       </c>
       <c r="G19" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B20" s="40">
         <v>12.4</v>
@@ -2733,12 +2721,12 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B21" s="40">
         <v>9.6</v>
@@ -2756,12 +2744,12 @@
         <v>1.4</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="38" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B22" s="40">
         <v>12.2</v>
@@ -2779,12 +2767,12 @@
         <v>1.8</v>
       </c>
       <c r="G22" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B23" s="40">
         <v>31.1</v>
@@ -2802,12 +2790,12 @@
         <v>6.3</v>
       </c>
       <c r="G23" s="40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="38" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B24" s="40">
         <v>12.2</v>
@@ -2825,7 +2813,7 @@
         <v>1.8</v>
       </c>
       <c r="G24" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2850,32 +2838,32 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="37" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C1" s="75" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D1" s="76"/>
       <c r="E1" s="76"/>
       <c r="F1" s="77"/>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="74"/>
       <c r="B2" s="29" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>34</v>
@@ -2890,9 +2878,9 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B3" s="32">
         <v>3.9300000000000002E-2</v>
@@ -2910,9 +2898,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B4" s="32">
         <v>3.7699999999999997E-2</v>
@@ -2930,9 +2918,9 @@
         <v>51.63</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B5" s="32">
         <v>3.7699999999999997E-2</v>
@@ -2950,9 +2938,9 @@
         <v>56.8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B6" s="32">
         <v>3.9300000000000002E-2</v>
@@ -2970,9 +2958,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B7" s="32">
         <v>3.9300000000000002E-2</v>
@@ -2990,9 +2978,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B8" s="32">
         <v>6.2899999999999998E-2</v>
@@ -3010,9 +2998,9 @@
         <v>56.56</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B9" s="32">
         <v>1.8100000000000002E-2</v>
@@ -3030,9 +3018,9 @@
         <v>37.08</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B10" s="32">
         <v>4.0000000000000001E-3</v>
@@ -3050,9 +3038,9 @@
         <v>234.05</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B11" s="32">
         <v>3.9E-2</v>
@@ -3070,12 +3058,12 @@
         <v>60.27</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C12" s="32">
         <v>51.4</v>
@@ -3090,9 +3078,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B13" s="32">
         <v>3.9E-2</v>
@@ -3110,9 +3098,9 @@
         <v>51.53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B14" s="32">
         <v>3.7699999999999997E-2</v>
@@ -3130,9 +3118,9 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B15" s="32">
         <v>3.7699999999999997E-2</v>
@@ -3150,9 +3138,9 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B16" s="32">
         <v>3.6999999999999998E-2</v>
@@ -3170,9 +3158,9 @@
         <v>6.43</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B17" s="32">
         <v>3.9300000000000002E-2</v>
@@ -3207,29 +3195,29 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="78" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B1" s="80" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C1" s="81"/>
     </row>
-    <row r="2" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="79"/>
       <c r="B2" s="47" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B3" s="49">
         <v>13.1</v>
@@ -3238,9 +3226,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B4" s="49">
         <v>4</v>
@@ -3249,9 +3237,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B5" s="49">
         <v>8.8000000000000007</v>
@@ -3260,9 +3248,9 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B6" s="49">
         <v>10.7</v>
@@ -3271,9 +3259,9 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B7" s="49">
         <v>4.0999999999999996</v>
@@ -3282,26 +3270,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C8" s="49" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="48" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -3325,15 +3313,15 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>28</v>
       </c>
@@ -3350,7 +3338,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
       <c r="B2" s="82"/>
       <c r="C2" s="85" t="s">
@@ -3363,7 +3351,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="83"/>
       <c r="B3" s="83"/>
       <c r="C3" s="88"/>
@@ -3372,10 +3360,10 @@
       <c r="F3" s="90"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>34</v>
@@ -3393,7 +3381,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
@@ -3416,7 +3404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
@@ -3439,9 +3427,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="24">
         <v>34.200000000000003</v>
@@ -3462,9 +3450,9 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" s="24">
         <v>33.1</v>
@@ -3485,9 +3473,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="1" customFormat="1" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="24">
         <v>37.5</v>
@@ -3508,9 +3496,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B10" s="24">
         <v>36.799999999999997</v>
@@ -3531,9 +3519,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="24">
         <v>37.299999999999997</v>
@@ -3554,9 +3542,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B12" s="24">
         <v>38.6</v>
@@ -3577,9 +3565,9 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="24">
         <v>39.700000000000003</v>
@@ -3600,9 +3588,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B14" s="24">
         <v>34.4</v>
@@ -3623,9 +3611,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" s="1" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B15" s="24">
         <v>34.4</v>
@@ -3646,9 +3634,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B16" s="24">
         <v>25.7</v>
@@ -3669,9 +3657,9 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" s="1" customFormat="1" ht="57.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="24">
         <v>31.4</v>
@@ -3692,9 +3680,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" s="24">
         <v>34.4</v>
@@ -3715,9 +3703,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B19" s="24">
         <v>34.6</v>
@@ -3735,12 +3723,12 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B20" s="24">
         <v>23.4</v>
@@ -3758,12 +3746,12 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B21" s="24">
         <v>23.4</v>
@@ -3781,14 +3769,14 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:7" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:A3"/>
@@ -3806,12 +3794,12 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="54" t="s">
         <v>28</v>
       </c>
@@ -3828,7 +3816,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="82"/>
       <c r="B2" s="82"/>
       <c r="C2" s="85" t="s">
@@ -3841,7 +3829,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="83"/>
       <c r="B3" s="83"/>
       <c r="C3" s="88"/>
@@ -3850,10 +3838,10 @@
       <c r="F3" s="90"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>34</v>
@@ -3871,12 +3859,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>42</v>
+      <c r="B5" s="24">
+        <v>45.3</v>
       </c>
       <c r="C5" s="12">
         <v>69.599999999999994</v>
@@ -3891,15 +3879,15 @@
         <v>69.88</v>
       </c>
       <c r="G5" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="24" t="s">
-        <v>45</v>
+      <c r="B6" s="24">
+        <v>46.5</v>
       </c>
       <c r="C6" s="25">
         <v>61</v>
@@ -3914,15 +3902,15 @@
         <v>61.28</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="B7" s="24">
+        <v>34.200000000000003</v>
       </c>
       <c r="C7" s="12">
         <v>92.6</v>
@@ -3940,12 +3928,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="B8" s="24">
+        <v>42.9</v>
       </c>
       <c r="C8" s="12">
         <v>54.7</v>
@@ -3963,12 +3951,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="B9" s="24">
+        <v>34.200000000000003</v>
       </c>
       <c r="C9" s="12">
         <v>92.6</v>
@@ -4009,14 +3997,14 @@
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>13</v>
       </c>
@@ -4027,7 +4015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -4038,7 +4026,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -4049,7 +4037,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -4060,7 +4048,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -4071,7 +4059,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -4082,7 +4070,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -4093,7 +4081,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -4104,7 +4092,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
@@ -4115,7 +4103,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
@@ -4126,7 +4114,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>25</v>
       </c>
@@ -4137,7 +4125,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -4148,7 +4136,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
@@ -4175,13 +4163,13 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -4189,7 +4177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -4197,7 +4185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -4205,7 +4193,7 @@
         <v>0.1229</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -4213,7 +4201,7 @@
         <v>0.3276</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -4221,7 +4209,7 @@
         <v>8.1900000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -4245,55 +4233,55 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B2" s="5">
         <v>0.879</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B4" s="5">
         <v>2.931</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B5" s="5">
         <v>1.649</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B6" s="5">
         <v>5.36</v>

</xml_diff>